<commit_message>
update alert added for capture
</commit_message>
<xml_diff>
--- a/logs/20-07-2020.xlsx
+++ b/logs/20-07-2020.xlsx
@@ -1720,7 +1720,11 @@
           <t>04:07:08</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr"/>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>05:45:42</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>